<commit_message>
working on code cleaning
</commit_message>
<xml_diff>
--- a/meta/21.03.29_Optimization Development Calculations_M.Ghodsvali.xlsx
+++ b/meta/21.03.29_Optimization Development Calculations_M.Ghodsvali.xlsx
@@ -5,19 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuenl-my.sharepoint.com/personal/m_ghodsvali_tue_nl/Documents/Collaboration/Papers/04-Decision Support System/MOO algorithm scripts/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuenl-my.sharepoint.com/personal/m_ghodsvali_tue_nl/Documents/Collaboration/Papers/04-Decision Support System/MOO algorithm scripts/Project/meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="8_{2974B8AF-CBE0-4A5C-B00A-27C9069D3009}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E3A781C0-8552-40D1-A3AF-46A8ADEA9BE3}"/>
+  <xr:revisionPtr revIDLastSave="76" documentId="8_{2974B8AF-CBE0-4A5C-B00A-27C9069D3009}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4CB895AB-7FFA-4461-94D0-2B74F378E810}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Socal acceptance (AHP)" sheetId="1" r:id="rId1"/>
     <sheet name="Compatibility" sheetId="2" r:id="rId2"/>
     <sheet name="Distance" sheetId="3" r:id="rId3"/>
     <sheet name="Standalone policy use" sheetId="5" r:id="rId4"/>
-    <sheet name="Possible policies combinations" sheetId="4" r:id="rId5"/>
+    <sheet name="Configs" sheetId="6" r:id="rId5"/>
+    <sheet name="Possible policies combinations" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="48">
   <si>
     <t>K1</t>
   </si>
@@ -180,6 +181,30 @@
   </si>
   <si>
     <t>Mixed-use</t>
+  </si>
+  <si>
+    <t>population</t>
+  </si>
+  <si>
+    <t>vegetable_demand</t>
+  </si>
+  <si>
+    <t>0.125*365</t>
+  </si>
+  <si>
+    <t>agri_land_availability</t>
+  </si>
+  <si>
+    <t>energy_land_availabilty</t>
+  </si>
+  <si>
+    <t>electricity_demand</t>
+  </si>
+  <si>
+    <t>error_buffer</t>
+  </si>
+  <si>
+    <t>grid_lenght</t>
   </si>
 </sst>
 </file>
@@ -2476,7 +2501,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B44EA1FC-CFB9-4FBB-9DED-2B39E11FE368}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -2623,6 +2648,81 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F664CE21-9435-45EE-BDCF-0A6862ECC5A2}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1">
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3">
+        <v>27000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4">
+        <v>140000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5">
+        <v>43200000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF9B36E7-9711-40D1-9FF3-AA0981DB91E2}">
   <dimension ref="A1:U13"/>
   <sheetViews>

</xml_diff>

<commit_message>
adding supply demand balance
</commit_message>
<xml_diff>
--- a/meta/21.03.29_Optimization Development Calculations_M.Ghodsvali.xlsx
+++ b/meta/21.03.29_Optimization Development Calculations_M.Ghodsvali.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuenl-my.sharepoint.com/personal/m_ghodsvali_tue_nl/Documents/Collaboration/Papers/04-Decision Support System/MOO algorithm scripts/Project/meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="217" documentId="8_{2974B8AF-CBE0-4A5C-B00A-27C9069D3009}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AF54828B-EF7F-4272-A645-490D13D549C8}"/>
+  <xr:revisionPtr revIDLastSave="220" documentId="8_{2974B8AF-CBE0-4A5C-B00A-27C9069D3009}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A0238B96-7D4C-41EA-B000-CE197FD43B7A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35400" yWindow="3675" windowWidth="17280" windowHeight="9075" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Distance" sheetId="3" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="64">
   <si>
     <t>K1</t>
   </si>
@@ -254,6 +254,9 @@
   </si>
   <si>
     <t>Policy</t>
+  </si>
+  <si>
+    <t>water_demand</t>
   </si>
 </sst>
 </file>
@@ -3243,9 +3246,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F664CE21-9435-45EE-BDCF-0A6862ECC5A2}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -3289,25 +3292,33 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="B5">
-        <v>43200000</v>
+        <v>122000</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>43200000</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>47</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>100</v>
       </c>
     </row>
@@ -3475,7 +3486,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67607632-E06E-4CE7-8149-E02E528F9800}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
small fix in supply_demand_balance function
</commit_message>
<xml_diff>
--- a/meta/21.03.29_Optimization Development Calculations_M.Ghodsvali.xlsx
+++ b/meta/21.03.29_Optimization Development Calculations_M.Ghodsvali.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuenl-my.sharepoint.com/personal/m_ghodsvali_tue_nl/Documents/Collaboration/Papers/04-Decision Support System/MOO algorithm scripts/Project/meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="220" documentId="8_{2974B8AF-CBE0-4A5C-B00A-27C9069D3009}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A0238B96-7D4C-41EA-B000-CE197FD43B7A}"/>
+  <xr:revisionPtr revIDLastSave="253" documentId="8_{2974B8AF-CBE0-4A5C-B00A-27C9069D3009}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3ACB0FF2-64BF-4775-A0D5-637857D7FB38}"/>
   <bookViews>
-    <workbookView xWindow="35400" yWindow="3675" windowWidth="17280" windowHeight="9075" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Distance" sheetId="3" r:id="rId1"/>
@@ -3249,7 +3249,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>